<commit_message>
Files and fixes added. Useless files removed.
</commit_message>
<xml_diff>
--- a/ConversionTracker.xlsx
+++ b/ConversionTracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Developer</t>
   </si>
@@ -61,6 +61,27 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>mAddDatatoSuptPoints</t>
+  </si>
+  <si>
+    <t>mDec2Bin</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Errors should be resolved after cSuptPoints will be added.</t>
+  </si>
+  <si>
+    <t>mAddRouteBranchesandOptions</t>
+  </si>
+  <si>
+    <t>mArchiveRun</t>
+  </si>
+  <si>
+    <t>mAssignSuptFrameSectionSizes</t>
   </si>
 </sst>
 </file>
@@ -148,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -167,6 +188,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -175,11 +199,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FF00CC00"/>
       <color rgb="FFFFFF00"/>
       <color rgb="FFFF0000"/>
       <color rgb="FFFF6600"/>
       <color rgb="FFCC0000"/>
-      <color rgb="FF00CC00"/>
       <color rgb="FF66FF66"/>
       <color rgb="FFFF5050"/>
     </mruColors>
@@ -480,10 +504,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -491,10 +515,11 @@
     <col min="1" max="1" width="17.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="44.44140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="71.109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -504,8 +529,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -515,8 +543,9 @@
       <c r="C2" s="4">
         <v>176</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -526,8 +555,9 @@
       <c r="C3" s="4">
         <v>155</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -537,8 +567,9 @@
       <c r="C4" s="4">
         <v>412</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -548,8 +579,9 @@
       <c r="C5" s="4">
         <v>355</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -559,8 +591,9 @@
       <c r="C6" s="4">
         <v>553</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
@@ -570,8 +603,9 @@
       <c r="C7" s="4">
         <v>226</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -581,8 +615,9 @@
       <c r="C8" s="4">
         <v>97</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -592,128 +627,182 @@
       <c r="C9" s="4">
         <v>563</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4">
+        <v>40</v>
+      </c>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="4">
+        <v>110</v>
+      </c>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4">
+        <v>77</v>
+      </c>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="5">
+        <v>502</v>
+      </c>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="5">
+        <v>54</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C15" s="5">
         <v>378</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C16" s="5">
         <v>217</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="3">
         <f>SUM(C2:C29)</f>
-        <v>3132</v>
-      </c>
+        <v>3915</v>
+      </c>
+      <c r="D30" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
More files and fixes added.
</commit_message>
<xml_diff>
--- a/ConversionTracker.xlsx
+++ b/ConversionTracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
   <si>
     <t>Developer</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Errors should be resolved after cSuptPoints will be added.</t>
-  </si>
-  <si>
     <t>mAddRouteBranchesandOptions</t>
   </si>
   <si>
@@ -82,6 +79,42 @@
   </si>
   <si>
     <t>mAssignSuptFrameSectionSizes</t>
+  </si>
+  <si>
+    <t>mBuildSupportFrameWorkOptions</t>
+  </si>
+  <si>
+    <t>mCalculateDirBasedonCoords</t>
+  </si>
+  <si>
+    <t>mCategoriseSuptpoints</t>
+  </si>
+  <si>
+    <t>mCollectLocalClashData</t>
+  </si>
+  <si>
+    <t>mExportColltoCSVFile</t>
+  </si>
+  <si>
+    <t>mExportArrtoCSVFile</t>
+  </si>
+  <si>
+    <t>mCreateAdjacentSuptpointsArray</t>
+  </si>
+  <si>
+    <t>mDirectionCheck</t>
+  </si>
+  <si>
+    <t>mCoordinateCheck</t>
+  </si>
+  <si>
+    <t>mDefinePerpsandParls</t>
+  </si>
+  <si>
+    <t>mCreateCoordArray</t>
+  </si>
+  <si>
+    <t>mDecomposeThreeDVectorintoENUCoords</t>
   </si>
 </sst>
 </file>
@@ -142,7 +175,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -165,11 +198,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -182,15 +228,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -504,10 +553,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -543,7 +592,7 @@
       <c r="C2" s="4">
         <v>176</v>
       </c>
-      <c r="D2" s="8"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -555,7 +604,7 @@
       <c r="C3" s="4">
         <v>155</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -567,7 +616,7 @@
       <c r="C4" s="4">
         <v>412</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -579,7 +628,7 @@
       <c r="C5" s="4">
         <v>355</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -591,7 +640,7 @@
       <c r="C6" s="4">
         <v>553</v>
       </c>
-      <c r="D6" s="8"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -603,7 +652,7 @@
       <c r="C7" s="4">
         <v>226</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -615,7 +664,7 @@
       <c r="C8" s="4">
         <v>97</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
@@ -627,7 +676,7 @@
       <c r="C9" s="4">
         <v>563</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -639,57 +688,55 @@
       <c r="C10" s="4">
         <v>40</v>
       </c>
-      <c r="D10" s="8"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="4">
         <v>110</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="4">
         <v>77</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="5">
         <v>502</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="5" t="s">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>54</v>
       </c>
-      <c r="D14" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
@@ -701,7 +748,7 @@
       <c r="C15" s="5">
         <v>378</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
@@ -713,100 +760,262 @@
       <c r="C16" s="5">
         <v>217</v>
       </c>
-      <c r="D16" s="8"/>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="A17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="5">
+        <v>175</v>
+      </c>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="A18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="4">
+        <v>111</v>
+      </c>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="A19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="5">
+        <v>162</v>
+      </c>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="A20" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="5">
+        <v>77</v>
+      </c>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="A21" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="4">
+        <v>76</v>
+      </c>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="A22" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="4">
+        <v>82</v>
+      </c>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="A23" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="4">
+        <v>107</v>
+      </c>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="A24" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="4">
+        <v>35</v>
+      </c>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
+      <c r="A25" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4">
+        <v>238</v>
+      </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="A26" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="4">
+        <v>65</v>
+      </c>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
+      <c r="A27" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="4">
+        <v>103</v>
+      </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="A28" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="4">
+        <v>114</v>
+      </c>
+      <c r="D28" s="11"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="11"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="3">
-        <f>SUM(C2:C29)</f>
-        <v>3915</v>
-      </c>
-      <c r="D30" s="3"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="6">
+        <f>SUM(C2:C44)</f>
+        <v>5260</v>
+      </c>
+      <c r="D45" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A45:B45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
added number of code lines to excel
</commit_message>
<xml_diff>
--- a/ConversionTracker.xlsx
+++ b/ConversionTracker.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>Developer</t>
   </si>
@@ -115,12 +115,33 @@
   </si>
   <si>
     <t>mDecomposeThreeDVectorintoENUCoords</t>
+  </si>
+  <si>
+    <t>Vahid</t>
+  </si>
+  <si>
+    <t>TubeDefDisc</t>
+  </si>
+  <si>
+    <t>cClashData</t>
+  </si>
+  <si>
+    <t>cLogEntry</t>
+  </si>
+  <si>
+    <t>cSteelDisc</t>
+  </si>
+  <si>
+    <t>cSuptPoints</t>
+  </si>
+  <si>
+    <t>cTubeDef</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -231,18 +252,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -261,14 +282,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -306,9 +330,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -343,7 +367,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -378,7 +402,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -555,8 +579,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -799,10 +823,10 @@
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="9" t="s">
+      <c r="A20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="5">
@@ -811,10 +835,10 @@
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="10" t="s">
+      <c r="A21" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="4">
@@ -823,10 +847,10 @@
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="10" t="s">
+      <c r="A22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="4">
@@ -835,10 +859,10 @@
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="10" t="s">
+      <c r="A23" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="8" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="4">
@@ -847,10 +871,10 @@
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="10" t="s">
+      <c r="A24" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="4">
@@ -859,10 +883,10 @@
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="10" t="s">
+      <c r="A25" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="4">
@@ -871,10 +895,10 @@
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="10" t="s">
+      <c r="A26" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="8" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="4">
@@ -883,10 +907,10 @@
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="10" t="s">
+      <c r="A27" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="4">
@@ -904,48 +928,90 @@
       <c r="C28" s="4">
         <v>114</v>
       </c>
-      <c r="D28" s="11"/>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="11"/>
+      <c r="A29" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="4">
+        <v>133</v>
+      </c>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="A30" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="4">
+        <v>52</v>
+      </c>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="A31" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="4">
+        <v>39</v>
+      </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="A32" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="4">
+        <v>275</v>
+      </c>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+      <c r="A33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="4">
+        <v>196</v>
+      </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
+      <c r="A34" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="4">
+        <v>399</v>
+      </c>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
+      <c r="A35" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="4">
+        <v>174</v>
+      </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1003,13 +1069,13 @@
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="8"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="6">
         <f>SUM(C2:C44)</f>
-        <v>5260</v>
+        <v>6528</v>
       </c>
       <c r="D45" s="3"/>
     </row>

</xml_diff>

<commit_message>
Files added. Resolved few errors.
</commit_message>
<xml_diff>
--- a/ConversionTracker.xlsx
+++ b/ConversionTracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
   <si>
     <t>Developer</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>mDecomposeThreeDVectorintoENUCoords</t>
+  </si>
+  <si>
+    <t>mGroupSimilarFrameNodes</t>
+  </si>
+  <si>
+    <t>mCollectLocalExistingDiscSteel</t>
   </si>
 </sst>
 </file>
@@ -215,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -231,15 +237,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -555,8 +560,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -799,22 +804,22 @@
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="9" t="s">
+      <c r="A20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>77</v>
       </c>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="10" t="s">
+      <c r="A21" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C21" s="4">
@@ -823,10 +828,10 @@
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="10" t="s">
+      <c r="A22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="4">
@@ -835,10 +840,10 @@
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" s="10" t="s">
+      <c r="A23" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="4">
@@ -847,10 +852,10 @@
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" s="10" t="s">
+      <c r="A24" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="4">
@@ -859,10 +864,10 @@
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="10" t="s">
+      <c r="A25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C25" s="4">
@@ -871,10 +876,10 @@
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" s="10" t="s">
+      <c r="A26" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C26" s="4">
@@ -883,10 +888,10 @@
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="10" t="s">
+      <c r="A27" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="4">
@@ -904,18 +909,30 @@
       <c r="C28" s="4">
         <v>114</v>
       </c>
-      <c r="D28" s="11"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="11"/>
+      <c r="A29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="4">
+        <v>680</v>
+      </c>
+      <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
+      <c r="A30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="4">
+        <v>275</v>
+      </c>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1003,13 +1020,13 @@
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="8"/>
+      <c r="B45" s="10"/>
       <c r="C45" s="6">
         <f>SUM(C2:C44)</f>
-        <v>5260</v>
+        <v>6215</v>
       </c>
       <c r="D45" s="3"/>
     </row>

</xml_diff>

<commit_message>
Files and some fixes added.
</commit_message>
<xml_diff>
--- a/ConversionTracker.xlsx
+++ b/ConversionTracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="47">
   <si>
     <t>Developer</t>
   </si>
@@ -121,13 +121,49 @@
   </si>
   <si>
     <t>mCollectLocalExistingDiscSteel</t>
+  </si>
+  <si>
+    <t>Vahid</t>
+  </si>
+  <si>
+    <t>TubeDefDisc</t>
+  </si>
+  <si>
+    <t>cClashData</t>
+  </si>
+  <si>
+    <t>cLogEntry</t>
+  </si>
+  <si>
+    <t>cSteelDisc</t>
+  </si>
+  <si>
+    <t>cSuptPoints</t>
+  </si>
+  <si>
+    <t>cTubeDef</t>
+  </si>
+  <si>
+    <t>mWriteLogFile</t>
+  </si>
+  <si>
+    <t>mWriteActivityLog</t>
+  </si>
+  <si>
+    <t>mTravelCurrRtandNdtoNextIntsctn</t>
+  </si>
+  <si>
+    <t>mConvertLocalXYZtoGlobal</t>
+  </si>
+  <si>
+    <t>mCorrectSuptFrameCoords</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,8 +196,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +219,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00CC00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -239,12 +293,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -254,8 +315,11 @@
   <colors>
     <mruColors>
       <color rgb="FF00CC00"/>
+      <color rgb="FFCCCCFF"/>
+      <color rgb="FFCC99FF"/>
+      <color rgb="FFFF0000"/>
+      <color rgb="FFFF9999"/>
       <color rgb="FFFFFF00"/>
-      <color rgb="FFFF0000"/>
       <color rgb="FFFF6600"/>
       <color rgb="FFCC0000"/>
       <color rgb="FF66FF66"/>
@@ -558,10 +622,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -936,15 +1000,27 @@
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
+      <c r="A31" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="4">
+        <v>49</v>
+      </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
+      <c r="A32" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="4">
+        <v>178</v>
+      </c>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -996,43 +1072,193 @@
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
+      <c r="A41" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="4">
+        <v>133</v>
+      </c>
+      <c r="D41" s="13"/>
+    </row>
+    <row r="42" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="4">
+        <v>52</v>
+      </c>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
+    <row r="43" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="4">
+        <v>39</v>
+      </c>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
+    <row r="44" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="4">
+        <v>275</v>
+      </c>
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45" s="4">
+        <v>196</v>
+      </c>
+      <c r="D45" s="13"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="4">
+        <v>399</v>
+      </c>
+      <c r="D46" s="13"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="4">
+        <v>174</v>
+      </c>
+      <c r="D47" s="13"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" s="4">
+        <v>12</v>
+      </c>
+      <c r="D48" s="13"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C49" s="4">
+        <v>40</v>
+      </c>
+      <c r="D49" s="13"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C50" s="5">
+        <v>39</v>
+      </c>
+      <c r="D50" s="13"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="13"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="13"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="13"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="13"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="13"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="6"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="6"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="6"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="6"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B45" s="10"/>
-      <c r="C45" s="6">
-        <f>SUM(C2:C44)</f>
-        <v>6215</v>
-      </c>
-      <c r="D45" s="3"/>
+      <c r="B60" s="11"/>
+      <c r="C60" s="9">
+        <f>SUM(C2:C59)</f>
+        <v>7801</v>
+      </c>
+      <c r="D60" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A60:B60"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
added some data manipulation
</commit_message>
<xml_diff>
--- a/ConversionTracker.xlsx
+++ b/ConversionTracker.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
   <si>
     <t>Developer</t>
   </si>
@@ -157,12 +157,36 @@
   </si>
   <si>
     <t>mCorrectSuptFrameCoords</t>
+  </si>
+  <si>
+    <t>mRedEntireStruModtoLocaltoTubi</t>
+  </si>
+  <si>
+    <t>mRoutePotentialSuptFrames</t>
+  </si>
+  <si>
+    <t>mRunClashandClearanceCheck</t>
+  </si>
+  <si>
+    <t>mRunInUserCreatedSuptPointsMode</t>
+  </si>
+  <si>
+    <t>mRunInUserDefinedPipeListMode</t>
+  </si>
+  <si>
+    <t>mSelectandDetailAncilliary</t>
+  </si>
+  <si>
+    <t>mSelectBestPotlSupt</t>
+  </si>
+  <si>
+    <t>mSelectBestSuptFrame</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -203,7 +227,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,6 +255,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,19 +326,19 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -330,14 +360,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -375,9 +408,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -412,7 +445,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,7 +480,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -624,8 +657,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1081,7 +1114,7 @@
       <c r="C41" s="4">
         <v>133</v>
       </c>
-      <c r="D41" s="13"/>
+      <c r="D41" s="10"/>
     </row>
     <row r="42" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
@@ -1129,7 +1162,7 @@
       <c r="C45" s="4">
         <v>196</v>
       </c>
-      <c r="D45" s="13"/>
+      <c r="D45" s="10"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
@@ -1141,7 +1174,7 @@
       <c r="C46" s="4">
         <v>399</v>
       </c>
-      <c r="D46" s="13"/>
+      <c r="D46" s="10"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
@@ -1153,7 +1186,7 @@
       <c r="C47" s="4">
         <v>174</v>
       </c>
-      <c r="D47" s="13"/>
+      <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
@@ -1165,7 +1198,7 @@
       <c r="C48" s="4">
         <v>12</v>
       </c>
-      <c r="D48" s="13"/>
+      <c r="D48" s="10"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
@@ -1177,66 +1210,114 @@
       <c r="C49" s="4">
         <v>40</v>
       </c>
-      <c r="D49" s="13"/>
+      <c r="D49" s="10"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B50" s="5" t="s">
+      <c r="A50" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="13">
         <v>39</v>
       </c>
-      <c r="D50" s="13"/>
+      <c r="D50" s="10"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="12"/>
-      <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="13"/>
+      <c r="A51" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" s="4">
+        <v>63</v>
+      </c>
+      <c r="D51" s="10"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="13"/>
+      <c r="A52" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" s="13">
+        <v>74</v>
+      </c>
+      <c r="D52" s="10"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="12"/>
-      <c r="B53" s="12"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="13"/>
+      <c r="A53" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C53" s="13">
+        <v>80</v>
+      </c>
+      <c r="D53" s="10"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="12"/>
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="13"/>
+      <c r="A54" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" s="13">
+        <v>61</v>
+      </c>
+      <c r="D54" s="10"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="12"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="13"/>
+      <c r="A55" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" s="13">
+        <v>112</v>
+      </c>
+      <c r="D55" s="10"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
+      <c r="A56" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C56" s="13">
+        <v>57</v>
+      </c>
       <c r="D56" s="3"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="6"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
+      <c r="A57" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C57" s="13">
+        <v>60</v>
+      </c>
       <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
+      <c r="A58" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B58" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C58" s="13">
+        <v>51</v>
+      </c>
       <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1246,13 +1327,13 @@
       <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="10" t="s">
+      <c r="A60" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B60" s="11"/>
+      <c r="B60" s="12"/>
       <c r="C60" s="9">
         <f>SUM(C2:C59)</f>
-        <v>7801</v>
+        <v>8359</v>
       </c>
       <c r="D60" s="3"/>
     </row>

</xml_diff>

<commit_message>
added more DataManipulation methods
</commit_message>
<xml_diff>
--- a/ConversionTracker.xlsx
+++ b/ConversionTracker.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
   <si>
     <t>Developer</t>
   </si>
@@ -216,12 +216,21 @@
   <si>
     <t>mCreateCompleteNodemap</t>
   </si>
+  <si>
+    <t>mRedEntireStruModtoLocal</t>
+  </si>
+  <si>
+    <t>mRedEntireStruDiscModtoLocal</t>
+  </si>
+  <si>
+    <t>mRationaliseBeamDefinitions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,8 +307,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -348,8 +364,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CC00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -398,11 +420,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -424,18 +470,30 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -448,21 +506,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -492,9 +544,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -532,9 +584,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -569,7 +621,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -604,7 +656,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -779,10 +831,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Worksheet____1"/>
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -795,16 +847,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="16" t="s">
         <v>16</v>
       </c>
     </row>
@@ -974,7 +1026,7 @@
       <c r="C15" s="4">
         <v>378</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="15" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1221,21 +1273,21 @@
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
+      <c r="A36" s="11"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="11"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
+      <c r="A37" s="11"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="13"/>
+      <c r="A38" s="11"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1275,11 +1327,11 @@
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="19">
+      <c r="B45" s="22"/>
+      <c r="C45" s="13">
         <f>SUM(C2:C44)</f>
         <v>7191</v>
       </c>
@@ -1508,121 +1560,133 @@
       <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="14"/>
-      <c r="B65" s="14"/>
-      <c r="C65" s="14"/>
+      <c r="A65" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C65" s="24">
+        <v>69</v>
+      </c>
       <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="14"/>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14"/>
+      <c r="A66" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B66" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" s="24">
+        <v>63</v>
+      </c>
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="14"/>
-      <c r="B67" s="14"/>
-      <c r="C67" s="14"/>
+      <c r="A67" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B67" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C67" s="24">
+        <v>156</v>
+      </c>
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="14"/>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
+      <c r="A68" s="12"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="12"/>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="14"/>
-      <c r="B69" s="14"/>
-      <c r="C69" s="14"/>
+      <c r="A69" s="12"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="12"/>
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="14"/>
-      <c r="B70" s="14"/>
-      <c r="C70" s="14"/>
+      <c r="A70" s="12"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="12"/>
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="14"/>
-      <c r="B71" s="14"/>
-      <c r="C71" s="14"/>
+      <c r="A71" s="12"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="12"/>
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="14"/>
-      <c r="B72" s="14"/>
-      <c r="C72" s="14"/>
+      <c r="A72" s="12"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="12"/>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="14"/>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
+      <c r="A73" s="12"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="14"/>
-      <c r="B74" s="14"/>
-      <c r="C74" s="14"/>
+      <c r="A74" s="12"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="14"/>
-      <c r="B75" s="14"/>
-      <c r="C75" s="14"/>
+      <c r="A75" s="12"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="14"/>
-      <c r="B76" s="14"/>
-      <c r="C76" s="14"/>
+      <c r="A76" s="12"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
       <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="14"/>
-      <c r="B77" s="14"/>
-      <c r="C77" s="14"/>
+      <c r="A77" s="12"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="12"/>
       <c r="D77" s="2"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="14"/>
-      <c r="B78" s="14"/>
-      <c r="C78" s="14"/>
+      <c r="A78" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B78" s="20"/>
+      <c r="C78" s="8">
+        <f>SUM(C47:C77)</f>
+        <v>2205</v>
+      </c>
       <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B79" s="16"/>
-      <c r="C79" s="8">
-        <f>SUM(C47:C78)</f>
-        <v>1917</v>
-      </c>
+      <c r="A79" s="5"/>
+      <c r="B79" s="5"/>
+      <c r="C79" s="5"/>
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="5"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="5"/>
+      <c r="A80" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B80" s="18"/>
+      <c r="C80" s="14">
+        <f>SUM(C45,C78)</f>
+        <v>9396</v>
+      </c>
       <c r="D80" s="2"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B81" s="12"/>
-      <c r="C81" s="20">
-        <f>SUM(C45,C79)</f>
-        <v>9108</v>
-      </c>
-      <c r="D81" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A78:B78"/>
     <mergeCell ref="A45:B45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added left vba objects to excel
</commit_message>
<xml_diff>
--- a/ConversionTracker.xlsx
+++ b/ConversionTracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="74">
   <si>
     <t>Developer</t>
   </si>
@@ -224,6 +224,33 @@
   </si>
   <si>
     <t>mRationaliseBeamDefinitions</t>
+  </si>
+  <si>
+    <t>mPopulateStartsinPotlFrameColl</t>
+  </si>
+  <si>
+    <t>mMasterSuptPointCreatorSub</t>
+  </si>
+  <si>
+    <t>mMasterFrameCreatorSub</t>
+  </si>
+  <si>
+    <t>mManipulateStrutoSupAFormat</t>
+  </si>
+  <si>
+    <t>mImportSDNFtoSupAFormat</t>
+  </si>
+  <si>
+    <t>mImportP3DSuptListtoSupA</t>
+  </si>
+  <si>
+    <t>mImportNavisClashtoSupA</t>
+  </si>
+  <si>
+    <t>mImportCSVFiletoColl</t>
+  </si>
+  <si>
+    <t>mIDPotTravelDirnsFromCENode</t>
   </si>
 </sst>
 </file>
@@ -315,7 +342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,6 +394,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00CC00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -448,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -511,6 +544,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -831,10 +870,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Worksheet____1"/>
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1351,7 +1390,7 @@
         <v>35</v>
       </c>
       <c r="C47" s="3">
-        <v>133</v>
+        <v>178</v>
       </c>
       <c r="D47" s="9"/>
     </row>
@@ -1363,7 +1402,7 @@
         <v>36</v>
       </c>
       <c r="C48" s="3">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="D48" s="2"/>
     </row>
@@ -1375,7 +1414,7 @@
         <v>37</v>
       </c>
       <c r="C49" s="3">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="D49" s="2"/>
     </row>
@@ -1387,7 +1426,7 @@
         <v>6</v>
       </c>
       <c r="C50" s="3">
-        <v>275</v>
+        <v>412</v>
       </c>
       <c r="D50" s="2"/>
     </row>
@@ -1399,7 +1438,7 @@
         <v>38</v>
       </c>
       <c r="C51" s="3">
-        <v>196</v>
+        <v>274</v>
       </c>
       <c r="D51" s="9"/>
     </row>
@@ -1411,7 +1450,7 @@
         <v>39</v>
       </c>
       <c r="C52" s="3">
-        <v>399</v>
+        <v>540</v>
       </c>
       <c r="D52" s="9"/>
     </row>
@@ -1423,7 +1462,7 @@
         <v>40</v>
       </c>
       <c r="C53" s="3">
-        <v>174</v>
+        <v>228</v>
       </c>
       <c r="D53" s="9"/>
     </row>
@@ -1435,7 +1474,7 @@
         <v>41</v>
       </c>
       <c r="C54" s="3">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="D54" s="9"/>
     </row>
@@ -1447,7 +1486,7 @@
         <v>42</v>
       </c>
       <c r="C55" s="3">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D55" s="9"/>
     </row>
@@ -1459,7 +1498,7 @@
         <v>43</v>
       </c>
       <c r="C56" s="10">
-        <v>39</v>
+        <v>134</v>
       </c>
       <c r="D56" s="9"/>
     </row>
@@ -1471,7 +1510,7 @@
         <v>46</v>
       </c>
       <c r="C57" s="3">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="D57" s="9"/>
     </row>
@@ -1483,7 +1522,7 @@
         <v>47</v>
       </c>
       <c r="C58" s="3">
-        <v>74</v>
+        <v>143</v>
       </c>
       <c r="D58" s="9"/>
     </row>
@@ -1495,7 +1534,7 @@
         <v>48</v>
       </c>
       <c r="C59" s="3">
-        <v>80</v>
+        <v>186</v>
       </c>
       <c r="D59" s="9"/>
     </row>
@@ -1507,7 +1546,7 @@
         <v>49</v>
       </c>
       <c r="C60" s="10">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="D60" s="9"/>
     </row>
@@ -1519,7 +1558,7 @@
         <v>50</v>
       </c>
       <c r="C61" s="10">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="D61" s="9"/>
     </row>
@@ -1567,7 +1606,7 @@
         <v>62</v>
       </c>
       <c r="C65" s="18">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="D65" s="2"/>
     </row>
@@ -1579,7 +1618,7 @@
         <v>63</v>
       </c>
       <c r="C66" s="18">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="D66" s="2"/>
     </row>
@@ -1591,102 +1630,174 @@
         <v>64</v>
       </c>
       <c r="C67" s="18">
-        <v>156</v>
+        <v>267</v>
       </c>
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="12"/>
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
+      <c r="A68" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B68" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" s="25">
+        <v>158</v>
+      </c>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="12"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="12"/>
+      <c r="A69" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B69" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C69" s="25">
+        <v>758</v>
+      </c>
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="12"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
+      <c r="A70" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B70" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" s="25">
+        <v>200</v>
+      </c>
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="12"/>
+      <c r="A71" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B71" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" s="25">
+        <v>120</v>
+      </c>
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="12"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
+      <c r="A72" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C72" s="25">
+        <v>261</v>
+      </c>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="12"/>
-      <c r="B73" s="12"/>
-      <c r="C73" s="12"/>
+      <c r="A73" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" s="25">
+        <v>37</v>
+      </c>
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="12"/>
-      <c r="B74" s="12"/>
-      <c r="C74" s="12"/>
+      <c r="A74" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" s="25">
+        <v>117</v>
+      </c>
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="12"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="12"/>
+      <c r="A75" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B75" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C75" s="25">
+        <v>73</v>
+      </c>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="12"/>
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
+      <c r="A76" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B76" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C76" s="25">
+        <v>77</v>
+      </c>
       <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="12"/>
-      <c r="B77" s="12"/>
-      <c r="C77" s="12"/>
+      <c r="B77" s="25"/>
+      <c r="C77" s="25"/>
       <c r="D77" s="2"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="21" t="s">
+      <c r="A78" s="12"/>
+      <c r="B78" s="25"/>
+      <c r="C78" s="25"/>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="12"/>
+      <c r="B79" s="25"/>
+      <c r="C79" s="25"/>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="12"/>
+      <c r="B80" s="12"/>
+      <c r="C80" s="12"/>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B78" s="22"/>
-      <c r="C78" s="8">
-        <f>SUM(C47:C77)</f>
-        <v>2205</v>
-      </c>
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="5"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="2"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="19" t="s">
+      <c r="B81" s="22"/>
+      <c r="C81" s="8">
+        <f>SUM(C47:C80)</f>
+        <v>5124</v>
+      </c>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="5"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B80" s="20"/>
-      <c r="C80" s="14">
-        <f>SUM(C45,C78)</f>
-        <v>9396</v>
-      </c>
-      <c r="D80" s="2"/>
+      <c r="B83" s="20"/>
+      <c r="C83" s="14">
+        <f>SUM(C45,C81)</f>
+        <v>12315</v>
+      </c>
+      <c r="D83" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A81:B81"/>
     <mergeCell ref="A45:B45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added all my files. Fixes added.
</commit_message>
<xml_diff>
--- a/ConversionTracker.xlsx
+++ b/ConversionTracker.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="85">
   <si>
     <t>Developer</t>
   </si>
@@ -180,9 +180,6 @@
     <t>mSelectBestSuptFrame</t>
   </si>
   <si>
-    <t>ExportFEMresults -&gt; YourWorkbookPath.xlsx</t>
-  </si>
-  <si>
     <t>Total Vahid:</t>
   </si>
   <si>
@@ -190,6 +187,96 @@
   </si>
   <si>
     <t>mCreateFEModelGeometry</t>
+  </si>
+  <si>
+    <t>mCreateExtendedBeams</t>
+  </si>
+  <si>
+    <t>mDefineSuptFramesSections</t>
+  </si>
+  <si>
+    <t>mCreateCompleteNodemap</t>
+  </si>
+  <si>
+    <t>mRedEntireStruModtoLocal</t>
+  </si>
+  <si>
+    <t>mRedEntireStruDiscModtoLocal</t>
+  </si>
+  <si>
+    <t>mRationaliseBeamDefinitions</t>
+  </si>
+  <si>
+    <t>mPopulateStartsinPotlFrameColl</t>
+  </si>
+  <si>
+    <t>mMasterSuptPointCreatorSub</t>
+  </si>
+  <si>
+    <t>mMasterFrameCreatorSub</t>
+  </si>
+  <si>
+    <t>mManipulateStrutoSupAFormat</t>
+  </si>
+  <si>
+    <t>mImportSDNFtoSupAFormat</t>
+  </si>
+  <si>
+    <t>mImportP3DSuptListtoSupA</t>
+  </si>
+  <si>
+    <t>mImportNavisClashtoSupA</t>
+  </si>
+  <si>
+    <t>mImportCSVFiletoColl</t>
+  </si>
+  <si>
+    <t>mIDPotTravelDirnsFromCENode</t>
+  </si>
+  <si>
+    <t>mCreateMinSuptBeams</t>
+  </si>
+  <si>
+    <t>mCreateTrimSteel</t>
+  </si>
+  <si>
+    <t>mCreateVerticalCols</t>
+  </si>
+  <si>
+    <t>mDefineMaxMajAxfromMinAxBeamD</t>
+  </si>
+  <si>
+    <t>mDetailSuptFrame</t>
+  </si>
+  <si>
+    <t>mDiscretiseBeamsforFrames</t>
+  </si>
+  <si>
+    <t>mFillterPotlSuptFramestoFeasible</t>
+  </si>
+  <si>
+    <t>mFindRotatedbyAngle</t>
+  </si>
+  <si>
+    <t>mFindSpecificPotlRoute</t>
+  </si>
+  <si>
+    <t>Added some logic into line 48 for converting float to float[] using CreateCoordArray method.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ExportFEMresults -&gt; YourWorkbookPath.xlsx. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Investigate OpenSTAAD.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -204,60 +291,38 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ExportFEMInput -&gt; YourWorkbookPath.xlsx</t>
+      <t>ExportFEMInput -&gt; YourWorkbookPath.xlsx.</t>
     </r>
   </si>
   <si>
-    <t>mCreateExtendedBeams</t>
-  </si>
-  <si>
-    <t>mDefineSuptFramesSections</t>
-  </si>
-  <si>
-    <t>mCreateCompleteNodemap</t>
-  </si>
-  <si>
-    <t>mRedEntireStruModtoLocal</t>
-  </si>
-  <si>
-    <t>mRedEntireStruDiscModtoLocal</t>
-  </si>
-  <si>
-    <t>mRationaliseBeamDefinitions</t>
-  </si>
-  <si>
-    <t>mPopulateStartsinPotlFrameColl</t>
-  </si>
-  <si>
-    <t>mMasterSuptPointCreatorSub</t>
-  </si>
-  <si>
-    <t>mMasterFrameCreatorSub</t>
-  </si>
-  <si>
-    <t>mManipulateStrutoSupAFormat</t>
-  </si>
-  <si>
-    <t>mImportSDNFtoSupAFormat</t>
-  </si>
-  <si>
-    <t>mImportP3DSuptListtoSupA</t>
-  </si>
-  <si>
-    <t>mImportNavisClashtoSupA</t>
-  </si>
-  <si>
-    <t>mImportCSVFiletoColl</t>
-  </si>
-  <si>
-    <t>mIDPotTravelDirnsFromCENode</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Should be fixed when mPopulateStartsinPotlFrameColl will be added. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GroupSimilarFrameNodes, PopulateStartsinPotlFrameColl, RoutePotentialSuptFrames: check OUT parameters.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,6 +404,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -503,9 +583,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -527,6 +604,12 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -545,15 +628,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -583,9 +661,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -623,9 +701,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -660,7 +738,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -695,7 +773,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -870,10 +948,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Worksheet____1"/>
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -886,16 +964,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1060,23 +1138,23 @@
         <v>3</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C15" s="4">
         <v>378</v>
       </c>
-      <c r="D15" s="15" t="s">
-        <v>54</v>
+      <c r="D15" s="14" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>217</v>
       </c>
       <c r="D16" s="5"/>
@@ -1091,7 +1169,9 @@
       <c r="C17" s="4">
         <v>175</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="26" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
@@ -1106,16 +1186,18 @@
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="4" t="s">
+      <c r="A19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C19" s="3">
         <v>162</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="26" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
@@ -1278,13 +1360,13 @@
         <v>3</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C33" s="4">
         <v>382</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1292,7 +1374,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C34" s="3">
         <v>180</v>
@@ -1304,7 +1386,7 @@
         <v>3</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C35" s="3">
         <v>187</v>
@@ -1312,68 +1394,117 @@
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
+      <c r="A36" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="3">
+        <v>202</v>
+      </c>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="11"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
+      <c r="A37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="3">
+        <v>372</v>
+      </c>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="11"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
+      <c r="A38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" s="3">
+        <v>277</v>
+      </c>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
+      <c r="A39" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C39" s="3">
+        <v>95</v>
+      </c>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
+      <c r="A40" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="3">
+        <v>693</v>
+      </c>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
+      <c r="A41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="3">
+        <v>99</v>
+      </c>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
+      <c r="A42" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="3">
+        <v>473</v>
+      </c>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
+      <c r="A43" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="3">
+        <v>29</v>
+      </c>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
+      <c r="A44" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="3">
+        <v>65</v>
+      </c>
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="13">
-        <f>SUM(C2:C44)</f>
-        <v>7191</v>
-      </c>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1383,98 +1514,85 @@
       <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B47" s="3" t="s">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="25"/>
+      <c r="C48" s="12">
+        <f>SUM(C2:C47)</f>
+        <v>9496</v>
+      </c>
+      <c r="D48" s="2"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C50" s="3">
         <v>178</v>
       </c>
-      <c r="D47" s="9"/>
-    </row>
-    <row r="48" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="3" t="s">
+      <c r="D50" s="9"/>
+    </row>
+    <row r="51" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C51" s="3">
         <v>108</v>
       </c>
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B49" s="3" t="s">
+      <c r="D51" s="2"/>
+    </row>
+    <row r="52" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C52" s="3">
         <v>77</v>
       </c>
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B50" s="3" t="s">
+      <c r="D52" s="2"/>
+    </row>
+    <row r="53" spans="1:4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C53" s="3">
         <v>412</v>
       </c>
-      <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C51" s="3">
-        <v>274</v>
-      </c>
-      <c r="D51" s="9"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C52" s="3">
-        <v>540</v>
-      </c>
-      <c r="D52" s="9"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53" s="3">
-        <v>228</v>
-      </c>
-      <c r="D53" s="9"/>
+      <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C54" s="3">
-        <v>55</v>
+        <v>274</v>
       </c>
       <c r="D54" s="9"/>
     </row>
@@ -1483,22 +1601,22 @@
         <v>34</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C55" s="3">
-        <v>43</v>
+        <v>540</v>
       </c>
       <c r="D55" s="9"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C56" s="10">
-        <v>134</v>
+      <c r="A56" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" s="3">
+        <v>228</v>
       </c>
       <c r="D56" s="9"/>
     </row>
@@ -1507,10 +1625,10 @@
         <v>34</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C57" s="3">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="D57" s="9"/>
     </row>
@@ -1519,46 +1637,46 @@
         <v>34</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C58" s="3">
+        <v>43</v>
+      </c>
+      <c r="D58" s="9"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" s="10">
+        <v>134</v>
+      </c>
+      <c r="D59" s="9"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C60" s="3">
+        <v>92</v>
+      </c>
+      <c r="D60" s="9"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C61" s="3">
         <v>143</v>
-      </c>
-      <c r="D58" s="9"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C59" s="3">
-        <v>186</v>
-      </c>
-      <c r="D59" s="9"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C60" s="10">
-        <v>106</v>
-      </c>
-      <c r="D60" s="9"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C61" s="10">
-        <v>148</v>
       </c>
       <c r="D61" s="9"/>
     </row>
@@ -1567,238 +1685,274 @@
         <v>34</v>
       </c>
       <c r="B62" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C62" s="3">
+        <v>186</v>
+      </c>
+      <c r="D62" s="9"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C63" s="10">
+        <v>106</v>
+      </c>
+      <c r="D63" s="9"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="10">
+        <v>148</v>
+      </c>
+      <c r="D64" s="9"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C65" s="3">
         <v>57</v>
       </c>
-      <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B63" s="3" t="s">
+      <c r="D65" s="2"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C66" s="3">
         <v>60</v>
       </c>
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B64" s="3" t="s">
+      <c r="D66" s="2"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C67" s="3">
         <v>51</v>
       </c>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B65" s="18" t="s">
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C68" s="17">
+        <v>82</v>
+      </c>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C69" s="17">
+        <v>82</v>
+      </c>
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B70" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="C65" s="18">
-        <v>82</v>
-      </c>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B66" s="18" t="s">
+      <c r="C70" s="17">
+        <v>267</v>
+      </c>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B71" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C66" s="18">
-        <v>82</v>
-      </c>
-      <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B67" s="18" t="s">
+      <c r="C71" s="18">
+        <v>158</v>
+      </c>
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="C67" s="18">
-        <v>267</v>
-      </c>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B68" s="25" t="s">
+      <c r="C72" s="18">
+        <v>758</v>
+      </c>
+      <c r="D72" s="2"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C68" s="25">
-        <v>158</v>
-      </c>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B69" s="25" t="s">
+      <c r="C73" s="18">
+        <v>200</v>
+      </c>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C69" s="25">
-        <v>758</v>
-      </c>
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B70" s="25" t="s">
+      <c r="C74" s="18">
+        <v>120</v>
+      </c>
+      <c r="D74" s="2"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B75" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="C70" s="25">
-        <v>200</v>
-      </c>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B71" s="25" t="s">
+      <c r="C75" s="18">
+        <v>261</v>
+      </c>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B76" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="C71" s="25">
-        <v>120</v>
-      </c>
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B72" s="25" t="s">
+      <c r="C76" s="18">
+        <v>37</v>
+      </c>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B77" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="25">
-        <v>261</v>
-      </c>
-      <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B73" s="25" t="s">
+      <c r="C77" s="18">
+        <v>117</v>
+      </c>
+      <c r="D77" s="2"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B78" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="C73" s="25">
-        <v>37</v>
-      </c>
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B74" s="25" t="s">
+      <c r="C78" s="18">
+        <v>73</v>
+      </c>
+      <c r="D78" s="2"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B79" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C74" s="25">
-        <v>117</v>
-      </c>
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B75" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C75" s="25">
-        <v>73</v>
-      </c>
-      <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B76" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="C76" s="25">
+      <c r="C79" s="18">
         <v>77</v>
       </c>
-      <c r="D76" s="2"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="12"/>
-      <c r="B77" s="25"/>
-      <c r="C77" s="25"/>
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="12"/>
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="12"/>
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="12"/>
-      <c r="B80" s="12"/>
-      <c r="C80" s="12"/>
+      <c r="A80" s="11"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="18"/>
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B81" s="22"/>
-      <c r="C81" s="8">
-        <f>SUM(C47:C80)</f>
+      <c r="A81" s="11"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="2"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="11"/>
+      <c r="B82" s="18"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="2"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="11"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B84" s="23"/>
+      <c r="C84" s="8">
+        <f>SUM(C50:C83)</f>
         <v>5124</v>
       </c>
-      <c r="D81" s="2"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="2"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="19" t="s">
+      <c r="D84" s="2"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="5"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="5"/>
+      <c r="D85" s="2"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B83" s="20"/>
-      <c r="C83" s="14">
-        <f>SUM(C45,C81)</f>
-        <v>12315</v>
-      </c>
-      <c r="D83" s="2"/>
+      <c r="B86" s="21"/>
+      <c r="C86" s="13">
+        <f>SUM(C48,C84)</f>
+        <v>14620</v>
+      </c>
+      <c r="D86" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A48:B48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Almost all fixes are done.
</commit_message>
<xml_diff>
--- a/ConversionTracker.xlsx
+++ b/ConversionTracker.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1" codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="89">
   <si>
     <t>Developer</t>
   </si>
@@ -279,8 +279,50 @@
     </r>
   </si>
   <si>
+    <t>ImportFlagTxt</t>
+  </si>
+  <si>
+    <t>mImportCSVFile</t>
+  </si>
+  <si>
+    <t>ExportFEMInput -&gt; YourWorkbookPath.xlsx.</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Should be fixed when mImportCSVFiletoColl will be added. </t>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>COMMENTED:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is NOT used in VBA project.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>COMMENTED:</t>
     </r>
     <r>
       <rPr>
@@ -291,47 +333,28 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ExportFEMInput -&gt; YourWorkbookPath.xlsx.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Should be fixed when mPopulateStartsinPotlFrameColl will be added. </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="9" tint="-0.249977111117893"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>GroupSimilarFrameNodes, PopulateStartsinPotlFrameColl, RoutePotentialSuptFrames: check OUT parameters.</t>
+      <t>is NOT used in VBA project.</t>
     </r>
   </si>
   <si>
-    <t>ImportFlagTxt</t>
-  </si>
-  <si>
-    <t>mImportCSVFile</t>
-  </si>
-  <si>
-    <t>Investigate</t>
+    <t>GroupSimilarFrameNodes, PopulateStartsinPotlFrameColl, RoutePotentialSuptFrames: check OUT//REF parameters.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,8 +453,25 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,12 +504,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFCC99FF"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -488,8 +522,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor rgb="FF99FF99"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -570,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -589,34 +623,37 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -635,27 +672,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
       <color rgb="FF00CC00"/>
+      <color rgb="FF99FF99"/>
+      <color rgb="FFCCFFCC"/>
       <color rgb="FFCC99FF"/>
       <color rgb="FFCCCCFF"/>
       <color rgb="FFFF0000"/>
@@ -663,8 +699,6 @@
       <color rgb="FFFFFF00"/>
       <color rgb="FFFF6600"/>
       <color rgb="FFCC0000"/>
-      <color rgb="FF66FF66"/>
-      <color rgb="FFFF5050"/>
     </mruColors>
   </colors>
   <extLst>
@@ -679,9 +713,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -719,9 +753,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -756,7 +790,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -791,7 +825,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -968,8 +1002,8 @@
   <sheetPr codeName="Worksheet____1"/>
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -982,16 +1016,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1161,7 +1195,7 @@
       <c r="C15" s="4">
         <v>378</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="13" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1178,17 +1212,17 @@
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="4" t="s">
+      <c r="A17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>175</v>
       </c>
-      <c r="D17" s="19" t="s">
-        <v>84</v>
+      <c r="D17" s="18" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -1213,7 +1247,7 @@
       <c r="C19" s="3">
         <v>162</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="18" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1374,17 +1408,17 @@
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="4" t="s">
+      <c r="A33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <v>382</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>83</v>
+      <c r="D33" s="27" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1520,10 +1554,18 @@
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="2"/>
+      <c r="A45" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" s="28">
+        <v>40</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
@@ -1538,13 +1580,13 @@
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="24" t="s">
+      <c r="A48" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B48" s="25"/>
-      <c r="C48" s="12">
+      <c r="B48" s="26"/>
+      <c r="C48" s="11">
         <f>SUM(C2:C47)</f>
-        <v>9496</v>
+        <v>9536</v>
       </c>
       <c r="D48" s="2"/>
     </row>
@@ -1663,17 +1705,17 @@
       <c r="D58" s="9"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B59" s="10" t="s">
+      <c r="A59" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="B59" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="C59" s="10">
-        <v>134</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>87</v>
+      <c r="C59" s="31">
+        <v>94</v>
+      </c>
+      <c r="D59" s="30" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1713,32 +1755,28 @@
       <c r="D62" s="9"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B63" s="10" t="s">
+      <c r="A63" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C63" s="10">
+      <c r="C63" s="3">
         <v>106</v>
       </c>
-      <c r="D63" s="9" t="s">
-        <v>87</v>
-      </c>
+      <c r="D63" s="9"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B64" s="10" t="s">
+      <c r="A64" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C64" s="10">
+      <c r="C64" s="3">
         <v>148</v>
       </c>
-      <c r="D64" s="9" t="s">
-        <v>87</v>
-      </c>
+      <c r="D64" s="9"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
@@ -1777,207 +1815,205 @@
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B68" s="17" t="s">
+      <c r="A68" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C68" s="17">
+      <c r="C68" s="16">
         <v>82</v>
       </c>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B69" s="17" t="s">
+      <c r="A69" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B69" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="C69" s="17">
+      <c r="C69" s="16">
         <v>82</v>
       </c>
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B70" s="17" t="s">
+      <c r="A70" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B70" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C70" s="17">
+      <c r="C70" s="16">
         <v>267</v>
       </c>
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B71" s="29" t="s">
+      <c r="A71" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B71" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C71" s="29">
+      <c r="C71" s="20">
         <v>158</v>
       </c>
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B72" s="29" t="s">
+      <c r="A72" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="C72" s="29">
+      <c r="C72" s="20">
         <v>758</v>
       </c>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B73" s="27" t="s">
+      <c r="A73" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B73" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="C73" s="27">
+      <c r="C73" s="20">
         <v>200</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>87</v>
-      </c>
+      <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B74" s="29" t="s">
+      <c r="A74" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B74" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C74" s="29">
+      <c r="C74" s="20">
         <v>120</v>
       </c>
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B75" s="29" t="s">
+      <c r="A75" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B75" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C75" s="29">
+      <c r="C75" s="20">
         <v>261</v>
       </c>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B76" s="29" t="s">
+      <c r="A76" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B76" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="C76" s="29">
+      <c r="C76" s="20">
         <v>37</v>
       </c>
       <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B77" s="29" t="s">
+      <c r="A77" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B77" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="C77" s="29">
+      <c r="C77" s="20">
         <v>117</v>
       </c>
       <c r="D77" s="2"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B78" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="C78" s="29">
+      <c r="A78" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B78" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C78" s="20">
         <v>44</v>
       </c>
       <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B79" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C79" s="29">
+      <c r="A79" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B79" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C79" s="20">
         <v>72</v>
       </c>
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B80" s="29" t="s">
+      <c r="A80" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B80" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C80" s="29">
+      <c r="C80" s="20">
         <v>73</v>
       </c>
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B81" s="29" t="s">
+      <c r="A81" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B81" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="C81" s="29">
+      <c r="C81" s="20">
         <v>77</v>
       </c>
       <c r="D81" s="2"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="11"/>
-      <c r="B82" s="18"/>
-      <c r="C82" s="18"/>
+      <c r="A82" s="10"/>
+      <c r="B82" s="17"/>
+      <c r="C82" s="17"/>
       <c r="D82" s="2"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="11"/>
-      <c r="B83" s="18"/>
-      <c r="C83" s="18"/>
+      <c r="A83" s="10"/>
+      <c r="B83" s="17"/>
+      <c r="C83" s="17"/>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="11"/>
-      <c r="B84" s="18"/>
-      <c r="C84" s="18"/>
+      <c r="A84" s="10"/>
+      <c r="B84" s="17"/>
+      <c r="C84" s="17"/>
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="11"/>
-      <c r="B85" s="11"/>
-      <c r="C85" s="11"/>
+      <c r="A85" s="10"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="10"/>
       <c r="D85" s="2"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="22" t="s">
+      <c r="A86" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="B86" s="23"/>
+      <c r="B86" s="24"/>
       <c r="C86" s="8">
         <f>SUM(C50:C85)</f>
-        <v>5240</v>
+        <v>5200</v>
       </c>
       <c r="D86" s="2"/>
     </row>
@@ -1988,11 +2024,11 @@
       <c r="D87" s="2"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="20" t="s">
+      <c r="A88" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B88" s="21"/>
-      <c r="C88" s="13">
+      <c r="B88" s="22"/>
+      <c r="C88" s="12">
         <f>SUM(C48,C86)</f>
         <v>14736</v>
       </c>

</xml_diff>